<commit_message>
Ubah konsep, hanya kelas karyawan (xls)
</commit_message>
<xml_diff>
--- a/Pemesanan Tiket Bioskop.xlsx
+++ b/Pemesanan Tiket Bioskop.xlsx
@@ -24,13 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
-  <si>
-    <t>Person</t>
-  </si>
-  <si>
-    <t>nama</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
   <si>
     <t>Film</t>
   </si>
@@ -38,9 +32,6 @@
     <t>namaFilm</t>
   </si>
   <si>
-    <t>alamat</t>
-  </si>
-  <si>
     <t>Studio</t>
   </si>
   <si>
@@ -54,9 +45,6 @@
   </si>
   <si>
     <t>hargaTiket</t>
-  </si>
-  <si>
-    <t>jabatan</t>
   </si>
   <si>
     <t>kdTransaksi</t>
@@ -139,12 +127,6 @@
     <t>generateKode()</t>
   </si>
   <si>
-    <t>addPerson()</t>
-  </si>
-  <si>
-    <t>showPerson()</t>
-  </si>
-  <si>
     <t>showFilm()</t>
   </si>
   <si>
@@ -170,20 +152,6 @@
   </si>
   <si>
     <t>addKaryawan()</t>
-  </si>
-  <si>
-    <r>
-      <t>Karyawan "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Segoe UI Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>is a" Person</t>
-    </r>
   </si>
   <si>
     <r>
@@ -198,6 +166,12 @@
       </rPr>
       <t>"has a" Studio</t>
     </r>
+  </si>
+  <si>
+    <t>Karyawan</t>
+  </si>
+  <si>
+    <t>namaKaryawan</t>
   </si>
 </sst>
 </file>
@@ -586,7 +560,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,7 +591,7 @@
     <row r="2" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="11" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
@@ -637,19 +611,19 @@
     <row r="4" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="10" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="10" t="s">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="10" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G4" s="2"/>
       <c r="I4" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
@@ -657,97 +631,95 @@
     <row r="5" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G5" s="2"/>
       <c r="I5" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K5" s="9">
         <v>865235482</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="2" t="s">
-        <v>4</v>
+      <c r="D6" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="6" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G6" s="2"/>
       <c r="I6" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="6" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G7" s="2"/>
       <c r="I7" s="4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="D8" s="7"/>
       <c r="E8" s="2"/>
       <c r="G8" s="2"/>
       <c r="I8" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
@@ -759,13 +731,13 @@
       <c r="F9" s="7"/>
       <c r="G9" s="2"/>
       <c r="I9" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="J9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="9" t="s">
         <v>23</v>
-      </c>
-      <c r="K9" s="9" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
@@ -777,10 +749,10 @@
       <c r="F10" s="7"/>
       <c r="G10" s="2"/>
       <c r="I10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="K10" s="9">
         <v>75000</v>
@@ -795,10 +767,10 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="I11" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K11" s="9">
         <v>2</v>
@@ -813,10 +785,10 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="I12" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K12" s="9">
         <v>150000</v>
@@ -825,102 +797,91 @@
     <row r="13" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="10" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="10" t="s">
-        <v>45</v>
-      </c>
       <c r="E13" s="2"/>
       <c r="F13" s="10" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="G13" s="2"/>
       <c r="I13" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C15" s="2"/>
-      <c r="D15" s="6" t="s">
-        <v>44</v>
-      </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C16" s="2"/>
-      <c r="D16" s="6" t="s">
-        <v>39</v>
-      </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G16" s="2"/>
+      <c r="I16" s="4"/>
     </row>
     <row r="17" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="7"/>
       <c r="E17" s="2"/>
       <c r="F17" s="6" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="7"/>
       <c r="E18" s="2"/>
       <c r="F18" s="6" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="7"/>

</xml_diff>

<commit_message>
Tambah Kelas Transaksi, yang disesuaikan
</commit_message>
<xml_diff>
--- a/Pemesanan Tiket Bioskop.xlsx
+++ b/Pemesanan Tiket Bioskop.xlsx
@@ -110,6 +110,42 @@
     <t>Kode film ditampilkan ketika program RUN</t>
   </si>
   <si>
+    <t>generateKode()</t>
+  </si>
+  <si>
+    <t>showFilm()</t>
+  </si>
+  <si>
+    <t>showStudio()</t>
+  </si>
+  <si>
+    <t>showJadwal()</t>
+  </si>
+  <si>
+    <t>showKaryawan()</t>
+  </si>
+  <si>
+    <t>showTransaksi()</t>
+  </si>
+  <si>
+    <t>addFilm()</t>
+  </si>
+  <si>
+    <t>addStudio()</t>
+  </si>
+  <si>
+    <t>addJadwal()</t>
+  </si>
+  <si>
+    <t>addKaryawan()</t>
+  </si>
+  <si>
+    <t>Karyawan</t>
+  </si>
+  <si>
+    <t>namaKaryawan</t>
+  </si>
+  <si>
     <r>
       <t>Transaksi "</t>
     </r>
@@ -120,58 +156,11 @@
         <rFont val="Segoe UI Light"/>
         <family val="2"/>
       </rPr>
-      <t>has a" Jadwal</t>
+      <t>is a" Jadwal</t>
     </r>
   </si>
   <si>
-    <t>generateKode()</t>
-  </si>
-  <si>
-    <t>showFilm()</t>
-  </si>
-  <si>
-    <t>showStudio()</t>
-  </si>
-  <si>
-    <t>showJadwal()</t>
-  </si>
-  <si>
-    <t>showKaryawan()</t>
-  </si>
-  <si>
-    <t>showTransaksi()</t>
-  </si>
-  <si>
-    <t>addFilm()</t>
-  </si>
-  <si>
-    <t>addStudio()</t>
-  </si>
-  <si>
-    <t>addJadwal()</t>
-  </si>
-  <si>
-    <t>addKaryawan()</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Jadwal </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Segoe UI Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>"has a" Studio</t>
-    </r>
-  </si>
-  <si>
-    <t>Karyawan</t>
-  </si>
-  <si>
-    <t>namaKaryawan</t>
+    <t>Jadwal</t>
   </si>
 </sst>
 </file>
@@ -214,7 +203,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -239,6 +228,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -252,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -276,6 +277,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -560,7 +567,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,7 +622,7 @@
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="10" t="s">
@@ -635,7 +642,7 @@
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
@@ -658,15 +665,15 @@
     <row r="6" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G6" s="2"/>
       <c r="I6" s="4" t="s">
@@ -675,7 +682,7 @@
       <c r="J6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="K6" s="13" t="s">
         <v>20</v>
       </c>
       <c r="M6" s="1" t="s">
@@ -685,15 +692,15 @@
     <row r="7" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G7" s="2"/>
       <c r="I7" s="4" t="s">
@@ -702,7 +709,7 @@
       <c r="J7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K7" s="9" t="s">
+      <c r="K7" s="13" t="s">
         <v>21</v>
       </c>
     </row>
@@ -718,7 +725,7 @@
       <c r="J8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="9" t="s">
+      <c r="K8" s="12" t="s">
         <v>22</v>
       </c>
     </row>
@@ -736,7 +743,7 @@
       <c r="J9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K9" s="9" t="s">
+      <c r="K9" s="12" t="s">
         <v>23</v>
       </c>
     </row>
@@ -754,7 +761,7 @@
       <c r="J10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K10" s="9">
+      <c r="K10" s="12">
         <v>75000</v>
       </c>
     </row>
@@ -772,7 +779,7 @@
       <c r="J11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K11" s="9">
+      <c r="K11" s="12">
         <v>2</v>
       </c>
     </row>
@@ -797,12 +804,12 @@
     <row r="13" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="10" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="C13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G13" s="2"/>
       <c r="I13" s="4" t="s">
@@ -861,27 +868,27 @@
       <c r="D17" s="7"/>
       <c r="E17" s="2"/>
       <c r="F17" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="7"/>
       <c r="E18" s="2"/>
       <c r="F18" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="7"/>

</xml_diff>